<commit_message>
small fix(saying truly not fix, just code update)
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -185,7 +185,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="n">
-        <v>94.0</v>
+        <v>92.0</v>
       </c>
       <c r="D5" t="n">
         <v>49185.0</v>
@@ -202,7 +202,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>92.0</v>
+        <v>90.0</v>
       </c>
       <c r="D6" t="n">
         <v>49185.0</v>
@@ -270,7 +270,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>93.0</v>
+        <v>91.0</v>
       </c>
       <c r="D10" t="n">
         <v>49185.0</v>
@@ -287,7 +287,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>91.0</v>
+        <v>89.0</v>
       </c>
       <c r="D11" t="n">
         <v>49185.0</v>
@@ -310,7 +310,7 @@
         <v>49185.0</v>
       </c>
       <c r="E12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -391,7 +391,7 @@
         <v>49185.0</v>
       </c>
       <c r="E3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -408,7 +408,7 @@
         <v>49185.0</v>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -436,7 +436,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>88.0</v>
+        <v>28.0</v>
       </c>
       <c r="D6" t="n">
         <v>49185.0</v>
@@ -493,7 +493,7 @@
         <v>49185.0</v>
       </c>
       <c r="E9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -504,7 +504,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>44.0</v>
+        <v>82.0</v>
       </c>
       <c r="D10" t="n">
         <v>49185.0</v>
@@ -521,7 +521,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>29.0</v>
+        <v>58.0</v>
       </c>
       <c r="D11" t="n">
         <v>49185.0</v>
@@ -589,7 +589,7 @@
         <v>9</v>
       </c>
       <c r="C15" t="n">
-        <v>83.0</v>
+        <v>89.0</v>
       </c>
       <c r="D15" t="n">
         <v>49185.0</v>
@@ -606,13 +606,13 @@
         <v>10</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0</v>
+        <v>65.0</v>
       </c>
       <c r="D16" t="n">
         <v>49185.0</v>
       </c>
       <c r="E16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -674,7 +674,7 @@
         <v>9</v>
       </c>
       <c r="C20" t="n">
-        <v>12.0</v>
+        <v>30.0</v>
       </c>
       <c r="D20" t="n">
         <v>49185.0</v>
@@ -691,7 +691,7 @@
         <v>10</v>
       </c>
       <c r="C21" t="n">
-        <v>87.0</v>
+        <v>27.0</v>
       </c>
       <c r="D21" t="n">
         <v>49185.0</v>
@@ -795,7 +795,7 @@
         <v>49187.0</v>
       </c>
       <c r="E2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -823,13 +823,13 @@
         <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>13.0</v>
+        <v>0.0</v>
       </c>
       <c r="D4" t="n">
         <v>49187.0</v>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -840,7 +840,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>88.0</v>
+        <v>28.0</v>
       </c>
       <c r="D5" t="n">
         <v>49187.0</v>
@@ -857,13 +857,13 @@
         <v>11</v>
       </c>
       <c r="C6" t="n">
-        <v>64.0</v>
+        <v>0.0</v>
       </c>
       <c r="D6" t="n">
         <v>49187.0</v>
       </c>
       <c r="E6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -908,7 +908,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="n">
-        <v>44.0</v>
+        <v>82.0</v>
       </c>
       <c r="D9" t="n">
         <v>49187.0</v>
@@ -925,13 +925,13 @@
         <v>10</v>
       </c>
       <c r="C10" t="n">
-        <v>29.0</v>
+        <v>0.0</v>
       </c>
       <c r="D10" t="n">
         <v>49187.0</v>
       </c>
       <c r="E10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -942,7 +942,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>14.0</v>
+        <v>44.0</v>
       </c>
       <c r="D11" t="n">
         <v>49187.0</v>
@@ -993,7 +993,7 @@
         <v>9</v>
       </c>
       <c r="C14" t="n">
-        <v>83.0</v>
+        <v>89.0</v>
       </c>
       <c r="D14" t="n">
         <v>49187.0</v>
@@ -1010,7 +1010,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>59.0</v>
+        <v>65.0</v>
       </c>
       <c r="D15" t="n">
         <v>49187.0</v>
@@ -1027,7 +1027,7 @@
         <v>11</v>
       </c>
       <c r="C16" t="n">
-        <v>45.0</v>
+        <v>83.0</v>
       </c>
       <c r="D16" t="n">
         <v>49187.0</v>
@@ -1078,7 +1078,7 @@
         <v>9</v>
       </c>
       <c r="C19" t="n">
-        <v>12.0</v>
+        <v>30.0</v>
       </c>
       <c r="D19" t="n">
         <v>49187.0</v>
@@ -1095,7 +1095,7 @@
         <v>10</v>
       </c>
       <c r="C20" t="n">
-        <v>87.0</v>
+        <v>27.0</v>
       </c>
       <c r="D20" t="n">
         <v>49187.0</v>
@@ -1112,7 +1112,7 @@
         <v>11</v>
       </c>
       <c r="C21" t="n">
-        <v>63.0</v>
+        <v>12.0</v>
       </c>
       <c r="D21" t="n">
         <v>49187.0</v>
@@ -1163,7 +1163,7 @@
         <v>9</v>
       </c>
       <c r="C24" t="n">
-        <v>31.0</v>
+        <v>60.0</v>
       </c>
       <c r="D24" t="n">
         <v>49187.0</v>
@@ -1216,7 +1216,7 @@
         <v>49191.0</v>
       </c>
       <c r="E2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -1227,13 +1227,13 @@
         <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>13.0</v>
+        <v>0.0</v>
       </c>
       <c r="D3" t="n">
         <v>49191.0</v>
       </c>
       <c r="E3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -1295,13 +1295,13 @@
         <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>58.0</v>
+        <v>0.0</v>
       </c>
       <c r="D7" t="n">
         <v>49191.0</v>
       </c>
       <c r="E7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1312,13 +1312,13 @@
         <v>11</v>
       </c>
       <c r="C8" t="n">
-        <v>44.0</v>
+        <v>0.0</v>
       </c>
       <c r="D8" t="n">
         <v>49191.0</v>
       </c>
       <c r="E8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1335,7 +1335,7 @@
         <v>49191.0</v>
       </c>
       <c r="E9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1352,7 +1352,7 @@
         <v>49191.0</v>
       </c>
       <c r="E10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1363,7 +1363,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>89.0</v>
+        <v>29.0</v>
       </c>
       <c r="D11" t="n">
         <v>49191.0</v>
@@ -1380,13 +1380,13 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>65.0</v>
+        <v>0.0</v>
       </c>
       <c r="D12" t="n">
         <v>49191.0</v>
       </c>
       <c r="E12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1431,7 +1431,7 @@
         <v>9</v>
       </c>
       <c r="C15" t="n">
-        <v>45.0</v>
+        <v>83.0</v>
       </c>
       <c r="D15" t="n">
         <v>49191.0</v>
@@ -1448,13 +1448,13 @@
         <v>11</v>
       </c>
       <c r="C16" t="n">
-        <v>30.0</v>
+        <v>0.0</v>
       </c>
       <c r="D16" t="n">
         <v>49191.0</v>
       </c>
       <c r="E16" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1471,7 +1471,7 @@
         <v>49191.0</v>
       </c>
       <c r="E17" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -1499,7 +1499,7 @@
         <v>9</v>
       </c>
       <c r="C19" t="n">
-        <v>87.0</v>
+        <v>27.0</v>
       </c>
       <c r="D19" t="n">
         <v>49191.0</v>
@@ -1516,7 +1516,7 @@
         <v>11</v>
       </c>
       <c r="C20" t="n">
-        <v>63.0</v>
+        <v>12.0</v>
       </c>
       <c r="D20" t="n">
         <v>49191.0</v>
@@ -1567,7 +1567,7 @@
         <v>9</v>
       </c>
       <c r="C23" t="n">
-        <v>31.0</v>
+        <v>60.0</v>
       </c>
       <c r="D23" t="n">
         <v>49191.0</v>
@@ -1584,7 +1584,7 @@
         <v>11</v>
       </c>
       <c r="C24" t="n">
-        <v>28.0</v>
+        <v>46.0</v>
       </c>
       <c r="D24" t="n">
         <v>49191.0</v>
@@ -1665,7 +1665,7 @@
         <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>90.0</v>
+        <v>88.0</v>
       </c>
       <c r="D4" t="n">
         <v>49187.0</v>
@@ -1682,7 +1682,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>88.0</v>
+        <v>95.0</v>
       </c>
       <c r="D5" t="n">
         <v>49187.0</v>
@@ -1699,7 +1699,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="n">
-        <v>95.0</v>
+        <v>93.0</v>
       </c>
       <c r="D6" t="n">
         <v>49187.0</v>
@@ -1750,7 +1750,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="n">
-        <v>89.0</v>
+        <v>96.0</v>
       </c>
       <c r="D9" t="n">
         <v>49187.0</v>
@@ -1767,7 +1767,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="n">
-        <v>96.0</v>
+        <v>94.0</v>
       </c>
       <c r="D10" t="n">
         <v>49187.0</v>
@@ -1784,7 +1784,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>94.0</v>
+        <v>92.0</v>
       </c>
       <c r="D11" t="n">
         <v>49187.0</v>
@@ -1824,7 +1824,7 @@
         <v>49187.0</v>
       </c>
       <c r="E13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1882,7 +1882,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>95.0</v>
+        <v>93.0</v>
       </c>
       <c r="D3" t="n">
         <v>49191.0</v>
@@ -1899,7 +1899,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>93.0</v>
+        <v>91.0</v>
       </c>
       <c r="D4" t="n">
         <v>49191.0</v>
@@ -1950,7 +1950,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>96.0</v>
+        <v>94.0</v>
       </c>
       <c r="D7" t="n">
         <v>49191.0</v>
@@ -1967,7 +1967,7 @@
         <v>11</v>
       </c>
       <c r="C8" t="n">
-        <v>94.0</v>
+        <v>92.0</v>
       </c>
       <c r="D8" t="n">
         <v>49191.0</v>
@@ -2018,7 +2018,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>88.0</v>
+        <v>95.0</v>
       </c>
       <c r="D11" t="n">
         <v>49191.0</v>
@@ -2035,7 +2035,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>95.0</v>
+        <v>93.0</v>
       </c>
       <c r="D12" t="n">
         <v>49191.0</v>
@@ -2105,7 +2105,7 @@
         <v>49185.0</v>
       </c>
       <c r="E2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -2122,7 +2122,7 @@
         <v>49185.0</v>
       </c>
       <c r="E3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -2139,7 +2139,7 @@
         <v>49185.0</v>
       </c>
       <c r="E4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -2150,7 +2150,7 @@
         <v>9</v>
       </c>
       <c r="C5" t="n">
-        <v>64.0</v>
+        <v>61.0</v>
       </c>
       <c r="D5" t="n">
         <v>49185.0</v>
@@ -2167,13 +2167,13 @@
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0</v>
+        <v>67.0</v>
       </c>
       <c r="D6" t="n">
         <v>49185.0</v>
       </c>
       <c r="E6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -2235,13 +2235,13 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>67.0</v>
+        <v>0.0</v>
       </c>
       <c r="D10" t="n">
         <v>49185.0</v>
       </c>
       <c r="E10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -2252,7 +2252,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>64.0</v>
+        <v>61.0</v>
       </c>
       <c r="D11" t="n">
         <v>49185.0</v>
@@ -2320,7 +2320,7 @@
         <v>9</v>
       </c>
       <c r="C15" t="n">
-        <v>61.0</v>
+        <v>67.0</v>
       </c>
       <c r="D15" t="n">
         <v>49185.0</v>
@@ -2373,7 +2373,7 @@
         <v>49187.0</v>
       </c>
       <c r="E2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -2390,7 +2390,7 @@
         <v>49187.0</v>
       </c>
       <c r="E3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -2401,13 +2401,13 @@
         <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>61.0</v>
+        <v>0.0</v>
       </c>
       <c r="D4" t="n">
         <v>49187.0</v>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -2418,7 +2418,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>67.0</v>
+        <v>64.0</v>
       </c>
       <c r="D5" t="n">
         <v>49187.0</v>
@@ -2435,7 +2435,7 @@
         <v>11</v>
       </c>
       <c r="C6" t="n">
-        <v>64.0</v>
+        <v>61.0</v>
       </c>
       <c r="D6" t="n">
         <v>49187.0</v>
@@ -2458,7 +2458,7 @@
         <v>49187.0</v>
       </c>
       <c r="E7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -2486,7 +2486,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="n">
-        <v>64.0</v>
+        <v>61.0</v>
       </c>
       <c r="D9" t="n">
         <v>49187.0</v>
@@ -2503,7 +2503,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="n">
-        <v>61.0</v>
+        <v>67.0</v>
       </c>
       <c r="D10" t="n">
         <v>49187.0</v>
@@ -2520,7 +2520,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>67.0</v>
+        <v>64.0</v>
       </c>
       <c r="D11" t="n">
         <v>49187.0</v>
@@ -2571,7 +2571,7 @@
         <v>9</v>
       </c>
       <c r="C14" t="n">
-        <v>67.0</v>
+        <v>64.0</v>
       </c>
       <c r="D14" t="n">
         <v>49187.0</v>
@@ -2588,7 +2588,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>64.0</v>
+        <v>61.0</v>
       </c>
       <c r="D15" t="n">
         <v>49187.0</v>
@@ -2652,13 +2652,13 @@
         <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>67.0</v>
+        <v>0.0</v>
       </c>
       <c r="D3" t="n">
         <v>49191.0</v>
       </c>
       <c r="E3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -2669,13 +2669,13 @@
         <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0</v>
+        <v>61.0</v>
       </c>
       <c r="D4" t="n">
         <v>49191.0</v>
       </c>
       <c r="E4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -2692,7 +2692,7 @@
         <v>49191.0</v>
       </c>
       <c r="E5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -2709,7 +2709,7 @@
         <v>49191.0</v>
       </c>
       <c r="E6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -2720,7 +2720,7 @@
         <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>64.0</v>
+        <v>61.0</v>
       </c>
       <c r="D7" t="n">
         <v>49191.0</v>
@@ -2737,7 +2737,7 @@
         <v>11</v>
       </c>
       <c r="C8" t="n">
-        <v>61.0</v>
+        <v>67.0</v>
       </c>
       <c r="D8" t="n">
         <v>49191.0</v>
@@ -2788,7 +2788,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>61.0</v>
+        <v>67.0</v>
       </c>
       <c r="D11" t="n">
         <v>49191.0</v>
@@ -2805,7 +2805,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>67.0</v>
+        <v>64.0</v>
       </c>
       <c r="D12" t="n">
         <v>49191.0</v>
@@ -2856,7 +2856,7 @@
         <v>9</v>
       </c>
       <c r="C15" t="n">
-        <v>67.0</v>
+        <v>64.0</v>
       </c>
       <c r="D15" t="n">
         <v>49191.0</v>
@@ -3039,13 +3039,13 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>44.0</v>
+        <v>0.0</v>
       </c>
       <c r="D10" t="n">
         <v>49185.0</v>
       </c>
       <c r="E10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -3056,13 +3056,13 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0</v>
+        <v>41.0</v>
       </c>
       <c r="D11" t="n">
         <v>49185.0</v>
       </c>
       <c r="E11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -3124,7 +3124,7 @@
         <v>9</v>
       </c>
       <c r="C15" t="n">
-        <v>53.0</v>
+        <v>52.0</v>
       </c>
       <c r="D15" t="n">
         <v>49185.0</v>
@@ -3141,7 +3141,7 @@
         <v>10</v>
       </c>
       <c r="C16" t="n">
-        <v>44.0</v>
+        <v>43.0</v>
       </c>
       <c r="D16" t="n">
         <v>49185.0</v>
@@ -3209,7 +3209,7 @@
         <v>9</v>
       </c>
       <c r="C20" t="n">
-        <v>36.0</v>
+        <v>35.0</v>
       </c>
       <c r="D20" t="n">
         <v>49185.0</v>
@@ -3226,7 +3226,7 @@
         <v>10</v>
       </c>
       <c r="C21" t="n">
-        <v>53.0</v>
+        <v>52.0</v>
       </c>
       <c r="D21" t="n">
         <v>49185.0</v>
@@ -3341,13 +3341,13 @@
         <v>11</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="D6" t="n">
         <v>49187.0</v>
       </c>
       <c r="E6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -3381,7 +3381,7 @@
         <v>49187.0</v>
       </c>
       <c r="E8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -3392,13 +3392,13 @@
         <v>9</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0</v>
+        <v>41.0</v>
       </c>
       <c r="D9" t="n">
         <v>49187.0</v>
       </c>
       <c r="E9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -3409,7 +3409,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="n">
-        <v>40.0</v>
+        <v>39.0</v>
       </c>
       <c r="D10" t="n">
         <v>49187.0</v>
@@ -3426,7 +3426,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="n">
-        <v>38.0</v>
+        <v>37.0</v>
       </c>
       <c r="D11" t="n">
         <v>49187.0</v>
@@ -3477,7 +3477,7 @@
         <v>9</v>
       </c>
       <c r="C14" t="n">
-        <v>44.0</v>
+        <v>43.0</v>
       </c>
       <c r="D14" t="n">
         <v>49187.0</v>
@@ -3494,7 +3494,7 @@
         <v>10</v>
       </c>
       <c r="C15" t="n">
-        <v>42.0</v>
+        <v>41.0</v>
       </c>
       <c r="D15" t="n">
         <v>49187.0</v>
@@ -3511,7 +3511,7 @@
         <v>11</v>
       </c>
       <c r="C16" t="n">
-        <v>40.0</v>
+        <v>39.0</v>
       </c>
       <c r="D16" t="n">
         <v>49187.0</v>
@@ -3551,7 +3551,7 @@
         <v>49187.0</v>
       </c>
       <c r="E18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -3562,13 +3562,13 @@
         <v>9</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0</v>
+        <v>52.0</v>
       </c>
       <c r="D19" t="n">
         <v>49187.0</v>
       </c>
       <c r="E19" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -3579,7 +3579,7 @@
         <v>10</v>
       </c>
       <c r="C20" t="n">
-        <v>44.0</v>
+        <v>43.0</v>
       </c>
       <c r="D20" t="n">
         <v>49187.0</v>
@@ -3596,7 +3596,7 @@
         <v>11</v>
       </c>
       <c r="C21" t="n">
-        <v>42.0</v>
+        <v>41.0</v>
       </c>
       <c r="D21" t="n">
         <v>49187.0</v>
@@ -3677,13 +3677,13 @@
         <v>11</v>
       </c>
       <c r="C4" t="n">
-        <v>36.0</v>
+        <v>0.0</v>
       </c>
       <c r="D4" t="n">
         <v>49191.0</v>
       </c>
       <c r="E4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -3717,7 +3717,7 @@
         <v>49191.0</v>
       </c>
       <c r="E6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -3785,7 +3785,7 @@
         <v>49191.0</v>
       </c>
       <c r="E10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -3796,7 +3796,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>53.0</v>
+        <v>52.0</v>
       </c>
       <c r="D11" t="n">
         <v>49191.0</v>
@@ -3813,13 +3813,13 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0</v>
+        <v>43.0</v>
       </c>
       <c r="D12" t="n">
         <v>49191.0</v>
       </c>
       <c r="E12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -3864,13 +3864,13 @@
         <v>9</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0</v>
+        <v>37.0</v>
       </c>
       <c r="D15" t="n">
         <v>49191.0</v>
       </c>
       <c r="E15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -3881,13 +3881,13 @@
         <v>11</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0</v>
+        <v>35.0</v>
       </c>
       <c r="D16" t="n">
         <v>49191.0</v>
       </c>
       <c r="E16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -3932,7 +3932,7 @@
         <v>9</v>
       </c>
       <c r="C19" t="n">
-        <v>42.0</v>
+        <v>41.0</v>
       </c>
       <c r="D19" t="n">
         <v>49191.0</v>
@@ -3949,7 +3949,7 @@
         <v>11</v>
       </c>
       <c r="C20" t="n">
-        <v>40.0</v>
+        <v>39.0</v>
       </c>
       <c r="D20" t="n">
         <v>49191.0</v>

</xml_diff>